<commit_message>
committing changes for CCDI automation 101525
</commit_message>
<xml_diff>
--- a/InputFiles/CCDI/TC01_CCDI_phs001327_Sex-Female_Race-White_diseasephs-NotReported.xlsx
+++ b/InputFiles/CCDI/TC01_CCDI_phs001327_Sex-Female_Race-White_diseasephs-NotReported.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatekaraa\Automation\08-25-25\Commons_Automation\InputFiles\CCDI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatekaraa\Automation\09-10-25\Commons_Automation\InputFiles\CCDI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770FB11B-D809-49F9-910F-85E5EDEE1ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54A5743-5273-43DF-B9EB-B664E32872A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -108,69 +108,88 @@
 left join funding f on s.study_id = f.study </t>
   </si>
   <si>
-    <t>with diagnosis1 as (
-select dgn."participant.id", group_concat(dgn.age_at_diagnosis,';') as age, group_concat(dgn.diagnosis,';') as diag,group_concat(dgn.anatomic_site,';') as ant_site from df_diagnosis dgn where dgn."participant.id" is not null group by dgn."participant.id" ),
-diagnosis2 as (select "participant.id",  group_concat(diagnosis,';') as diag from (select distinct "participant.id", diagnosis from df_diagnosis  where "participant.id" is not null )  group by "participant.id" ),
-diagnosis3 as (select "participant.id",  group_concat(anatomic_site,';') as ant_site from (select distinct "participant.id", anatomic_site from df_diagnosis where "participant.id" is not null ) group by "participant.id" ),
-diagnosis4 as (
-  select distinct "participant.id", diagnosis, disease_phase
-  from df_diagnosis
-  where "participant.id" is not null
+    <t>WITH file_data AS (
+  SELECT
+    file_name, data_category, file_description, file_type, file_size, file_access,
+    "sample.id"
+  FROM df_sequencing_file
 )
 SELECT DISTINCT
+    fd.file_name AS "File Name",
+    REPLACE(fd.data_category, ';', ', ') AS "Data Category",
+    COALESCE(fd.file_description, '') AS "File Description",
+    fd.file_type AS "File Type",
+    CASE
+      WHEN fd.file_size &gt;= 1024 * 1024 * 1024 THEN 
+        CASE 
+          WHEN ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 2) = CAST(ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 0) AS INT) 
+          THEN CAST(CAST(ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 0) AS INT) AS TEXT) || ' GB'
+          ELSE ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 2) || ' GB'
+        END
+      WHEN fd.file_size &gt;= 1024 * 1024 THEN 
+        CASE 
+          WHEN ROUND(fd.file_size / (1024.0 * 1024.0), 2) = CAST(ROUND(fd.file_size / (1024.0 * 1024.0), 0) AS INT) 
+          THEN CAST(CAST(ROUND(fd.file_size / (1024.0 * 1024.0), 0) AS INT) AS TEXT) || ' MB'
+          ELSE ROUND(fd.file_size / (1024.0 * 1024.0), 2) || ' MB'
+        END
+      WHEN fd.file_size &gt;= 1024 THEN 
+        CASE 
+          WHEN ROUND(fd.file_size / 1024.0, 2) = CAST(ROUND(fd.file_size / 1024.0, 0) AS INT) 
+          THEN CAST(CAST(ROUND(fd.file_size / 1024.0, 0) AS INT) AS TEXT) || ' KB'
+          ELSE ROUND(fd.file_size / 1024.0, 2) || ' KB'
+        END
+      ELSE 
+        CASE 
+          WHEN ROUND(fd.file_size, 2) = CAST(ROUND(fd.file_size, 0) AS INT) 
+          THEN CAST(CAST(ROUND(fd.file_size, 0) AS INT) AS TEXT) || ' Bytes'
+          ELSE ROUND(fd.file_size, 2) || ' Bytes'
+        END
+    END AS "File Size",
+    fd.file_access AS "File Access",
+    std.dbgap_accession AS "Study ID",
     prt.participant_id AS "Participant ID",
-    std.dbgap_accession AS "Study ID",
-    COALESCE(prt.sex_at_birth, '') AS "Sex",
-    COALESCE(prt.race, '') AS "Race",
-	dgn2.diag AS "Diagnosis",
-	dgn3.ant_site AS "Diagnosis Anatomic Site",
-CASE
-        WHEN dgn."participant.id" IS NOT NULL THEN dgn.diagnosis_category 
-        ELSE NULL
-    END AS "Diagnosis_Category",
-	   COALESCE(CASE WHEN dgn1.age = '-999' THEN 'Not Reported' ELSE dgn1.age END, "") AS "Age at Diagnosis (days)",
-	null AS "Treatment Type",
-	srv.last_known_survival_status AS "Last Known Survival Status"
-FROM 
-    df_study std
-LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    diagnosis1 dgn1 ON prt.id = dgn1."participant.id" 
-LEFT JOIN 
-    diagnosis2 dgn2 ON prt.id = dgn2."participant.id"
-LEFT JOIN 
-    diagnosis3 dgn3 ON prt.id = dgn3."participant.id"
-LEFT JOIN 
-    diagnosis4 dgn4 ON prt.id = dgn4."participant.id"
-LEFT JOIN 
-    df_survival srv ON prt.id = srv."participant.id"
+    smp.sample_id AS "Sample ID"
+FROM df_study std
+LEFT JOIN df_consent_group  cg  ON std.id = cg."study.id"
+LEFT JOIN df_participant    prt ON cg.id  = prt."consent_group.id"
+LEFT JOIN df_sample         smp ON prt.id = smp."participant.id"
+JOIN      file_data         fd  ON smp.id = fd."sample.id"
+LEFT JOIN df_diagnosis      diag ON prt.id = diag."participant.id"
+LEFT JOIN df_sequencing_file seq ON smp.id = seq."sample.id"
+LEFT JOIN df_survival       sur  ON prt.id = sur."participant.id"
 WHERE 
-    std.dbgap_accession = 'phs001327' and prt.sex_at_birth ='Female' and prt.race LIKE '%White%' and dgn4.disease_phase = 'Not Reported'
-ORDER BY 
-    prt.participant_id ASC 
-;</t>
+  std.dbgap_accession = 'phs001327'
+AND prt.sex_at_birth = 'Female'
+   AND prt.race LIKE '%White%'
+  AND diag.disease_phase = 'Not Reported' 
+ORDER BY fd.file_name
+LIMIT 100;</t>
   </si>
   <si>
     <t>SELECT
     COUNT(DISTINCT std.dbgap_accession) AS "Studies",
     COUNT(DISTINCT prt.participant_id) AS "Participants",
     COUNT(DISTINCT smp.sample_id) AS "Samples",
-    (COUNT(DISTINCT seq.id) + COUNT(DISTINCT path.id)) AS "Files"
+    COUNT(DISTINCT seq.id) AS "Files"
 FROM 
     df_study std
 LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
+    df_consent_group  cg ON std.id = cg."study.id"
+LEFT JOIN 
+    df_participant prt ON cg.id = prt."consent_group.id"
 LEFT JOIN 
     df_sample smp ON prt.id = smp."participant.id"
 LEFT JOIN 
     df_sequencing_file seq ON smp.id = seq."sample.id"
-LEFT JOIN 
-    df_pathology_file path ON smp.id = path."sample.id"
-LEFT JOIN 
-  df_diagnosis dgn ON prt.id = dgn."participant.id"
+Left Join
+   df_diagnosis dgn On prt.id = dgn."participant.id"
+Left Join
+   df_survival sur On prt.id = sur."participant.id"
 WHERE 
-    std.dbgap_accession = 'phs001327' and prt.sex_at_birth = 'Female' and prt.race LIKE '%White%' and dgn.disease_phase = 'Not Reported';</t>
+ std.dbgap_accession = 'phs001327'
+	and dgn.diagnosis = 'Sarcoma, NOS'
+	and smp.anatomic_site = 'C42.0 : Blood'
+	and prt.sex_at_birth = 'Male';</t>
   </si>
   <si>
     <t>SELECT DISTINCT
@@ -187,118 +206,94 @@
     ) AS "Age at Sample Collection (days)",
     COALESCE(smp.sample_tumor_status, '') AS "Sample Tumor Status",
     COALESCE(smp.tumor_classification, '') AS "Sample Tumor Classification",
-    Null AS "Sample Diagnosis",
-CASE
+     CASE
+        WHEN dgn."sample.id" IS NOT NULL THEN dgn.diagnosis
+        ELSE NULL
+    END AS "Sample Diagnosis",
+	COALESCE 
+	(CASE
         WHEN dgn."sample.id" IS NOT NULL THEN dgn.diagnosis_category 
         ELSE NULL
-    END AS "Diagnosis_Category"
-FROM 
-    df_study std
-LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    df_sample smp ON prt.id = smp."participant.id"
-LEFT JOIN 
-    df_diagnosis dgn ON prt.id = dgn."participant.id"
-LEFT JOIN 
-    df_survival srv ON prt.id = srv."participant.id"
+    END,'') AS "Diagnosis_Category"
+FROM df_study std
+LEFT JOIN df_consent_group  cg ON std.id = cg."study.id"
+LEFT JOIN df_participant prt ON cg.id = prt."consent_group.id"
+LEFT JOIN df_sample smp ON prt.id = smp."participant.id"
+LEFT JOIN df_diagnosis dgn ON prt.id = dgn."participant.id"
+LEFT JOIN df_survival srv ON prt.id = srv."participant.id"
+LEFT JOIN df_sequencing_file seq ON smp.id = seq."sample.id"
 WHERE 
-    std.dbgap_accession = 'phs001327' 
-    AND prt.sex_at_birth = 'Female'
-   AND prt.race LIKE '%White%'
-   AND dgn.disease_phase = 'Not Reported' 
-    AND smp.sample_id IS NOT NULL
-ORDER BY 
-    smp.sample_id ASC;</t>
-  </si>
-  <si>
-    <t>WITH file_data AS (
+ std.dbgap_accession = 'phs001327'
+	and dgn.diagnosis = 'Sarcoma, NOS'
+	and smp.anatomic_site = 'C42.0 : Blood'
+	and prt.sex_at_birth = 'Male'
+ORDER BY smp.sample_id ASC
+Limit 100;</t>
+  </si>
+  <si>
+    <t>WITH diagnosis_summary AS ( 
     SELECT 
-        file_name, 
-        data_category,
-        file_type, 
-        file_size,
-        file_access,  
-        file_description,
-        "sample.id",
-        'Sequencing' AS file_source
-    FROM df_sequencing_file
-    UNION
+        dgn."participant.id" AS participant_id, 
+        GROUP_CONCAT(DISTINCT dgn.age_at_diagnosis) AS age_at_diagnosis, 
+        GROUP_CONCAT(DISTINCT dgn.diagnosis) AS diagnosis, 
+        GROUP_CONCAT(DISTINCT dgn.anatomic_site) AS anatomic_site,
+        GROUP_CONCAT(DISTINCT dgn.diagnosis_category) AS diagnosis_category
+    FROM df_diagnosis dgn
+    WHERE dgn."participant.id" IS NOT NULL
+    GROUP BY dgn."participant.id"
+),
+survival_summary AS (
     SELECT 
-        file_name, 
-        data_category,
-        file_type, 
-        file_size,
-        file_access,  
-        file_description,
-        "sample.id",
-        'Pathology' AS file_source
-    FROM df_pathology_file
+        "participant.id" AS participant_id,
+        GROUP_CONCAT(DISTINCT last_known_survival_status) AS last_known_survival_status
+    FROM df_survival
+    GROUP BY "participant.id"
+),
+sequencing_summary AS (
+    SELECT 
+        smp."participant.id" AS participant_id,
+        GROUP_CONCAT(DISTINCT smp.anatomic_site) AS sample_anatomic_sites,
+        GROUP_CONCAT(DISTINCT seq.library_strategy) AS library_strategies
+    FROM df_sample smp
+    LEFT JOIN df_sequencing_file seq ON smp.id = seq."sample.id"
+    GROUP BY smp."participant.id"
 )
-SELECT DISTINCT
-    fd.file_name AS "File Name",
-    fd.data_category AS "Data Category",
-    COALESCE(fd.file_description, '') AS "File Description",
-    fd.file_type AS "File Type",
-    CASE
-        WHEN fd.file_size &gt;= 1024 * 1024 * 1024 THEN
-            CASE 
-                WHEN ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 2) = CAST(ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 0) AS INT)
-                THEN CAST(CAST(ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 0) AS INT) AS TEXT) || ' GB'
-                ELSE ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 2) || ' GB'
-            END
-        WHEN fd.file_size &gt;= 1024 * 1024 THEN
-            CASE 
-                WHEN ROUND(fd.file_size / (1024.0 * 1024.0), 2) = CAST(ROUND(fd.file_size / (1024.0 * 1024.0), 0) AS INT)
-                THEN CAST(CAST(ROUND(fd.file_size / (1024.0 * 1024.0), 0) AS INT) AS TEXT) || ' MB'
-                ELSE ROUND(fd.file_size / (1024.0 * 1024.0), 2) || ' MB'
-            END
-        WHEN fd.file_size &gt;= 1024 THEN
-            CASE 
-                WHEN ROUND(fd.file_size / 1024.0, 2) = CAST(ROUND(fd.file_size / 1024.0, 0) AS INT)
-                THEN CAST(CAST(ROUND(fd.file_size / 1024.0, 0) AS INT) AS TEXT) || ' KB'
-                ELSE ROUND(fd.file_size / 1024.0, 2) || ' KB'
-            END
-        ELSE 
-            CASE 
-                WHEN ROUND(fd.file_size, 2) = CAST(ROUND(fd.file_size, 0) AS INT)
-                THEN CAST(CAST(ROUND(fd.file_size, 0) AS INT) AS TEXT) || ' Bytes'
-                ELSE ROUND(fd.file_size, 2) || ' Bytes'
-            END
-    END AS "File Size",
-    fd.file_access AS "File Access",
+SELECT
+    prt.participant_id AS "Participant ID",
     std.dbgap_accession AS "Study ID",
-    prt.participant_id AS "Participant ID",
-    smp.sample_id AS "Sample ID"
-  FROM 
-    df_study std
-LEFT JOIN df_participant prt ON std.id = prt."study.id"
-LEFT JOIN df_sample smp ON prt.id = smp."participant.id"
-JOIN file_data fd ON smp.id = fd."sample.id"
-LEFT JOIN df_diagnosis dgn ON prt.id = dgn."participant.id"
+    COALESCE(prt.sex_at_birth, '') AS "Sex",
+    COALESCE(prt.race, '') AS "Race",
+    COALESCE(dgn.diagnosis, '') AS "Diagnosis",
+    COALESCE(dgn.anatomic_site, '') AS "Diagnosis Anatomic Site",
+    COALESCE(
+        CASE WHEN dgn.participant_id IS NOT NULL THEN dgn.diagnosis_category END, ''
+    ) AS "Diagnosis_Category",
+    COALESCE(
+        CASE WHEN dgn.age_at_diagnosis = '-999' THEN 'Not Reported' ELSE dgn.age_at_diagnosis END, ''
+    ) AS "Age at Diagnosis (days)",
+    NULL AS "Treatment Type",
+    COALESCE(srv.last_known_survival_status, '') AS "Last Known Survival Status"
+FROM df_study std
+LEFT JOIN df_consent_group  cg    ON std.id = cg."study.id"
+LEFT JOIN df_participant    prt   ON cg.id  = prt."consent_group.id"
+LEFT JOIN diagnosis_summary dgn   ON prt.id = dgn.participant_id
+LEFT JOIN survival_summary  srv   ON prt.id = srv.participant_id
+LEFT JOIN sequencing_summary seqsum ON prt.id = seqsum.participant_id
 WHERE 
     std.dbgap_accession = 'phs001327'
-    AND prt.sex_at_birth = 'Female'
-    AND prt.race LIKE '%White%'
-    AND dgn.disease_phase = 'Not Reported'
-ORDER BY fd.file_name 
-LIMIT 100;</t>
+    AND dgn.diagnosis = 'Atypical Meningioma'
+    AND seqsum.sample_anatomic_sites = 'C71.9 : Brain, NOS' 
+    AND prt.sex_at_birth = 'Male'
+ORDER BY prt.participant_id ASC;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -324,13 +319,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -351,17 +339,11 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -684,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,10 +699,10 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
@@ -734,16 +716,16 @@
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="2"/>
@@ -752,8 +734,8 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>15</v>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -765,7 +747,7 @@
       <c r="C7" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>